<commit_message>
Aded env image + updated excel points sheet
</commit_message>
<xml_diff>
--- a/downloads/2023_DRAFT_Points_and_Penaltys_and_Tasks.xlsx
+++ b/downloads/2023_DRAFT_Points_and_Penaltys_and_Tasks.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="130">
   <si>
     <t xml:space="preserve">RoboCup At Work Pointsystem</t>
   </si>
@@ -202,16 +202,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">-&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">A successful </t>
+      <t xml:space="preserve">-&gt; A successful </t>
     </r>
     <r>
       <rPr>
@@ -220,6 +211,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cavity Placement</t>
     </r>
@@ -229,6 +221,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> = 200 points</t>
     </r>
@@ -245,16 +238,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">-&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">A successful </t>
+      <t xml:space="preserve">-&gt; A successful </t>
     </r>
     <r>
       <rPr>
@@ -263,6 +247,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Precision Placement</t>
     </r>
@@ -272,6 +257,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> = 300 points</t>
     </r>
@@ -431,15 +417,6 @@
     <t xml:space="preserve">Environment Decisions</t>
   </si>
   <si>
-    <t xml:space="preserve">BTT3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Objects
 Decoys</t>
   </si>
@@ -450,12 +427,12 @@
     <t xml:space="preserve">REF</t>
   </si>
   <si>
+    <t xml:space="preserve">Rotation</t>
+  </si>
+  <si>
     <t xml:space="preserve">TEAM</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Orientation</t>
   </si>
   <si>
@@ -468,9 +445,15 @@
     <t xml:space="preserve">0cm, 5cm, 10cm, 15cm</t>
   </si>
   <si>
+    <t xml:space="preserve">RTT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rotation direction</t>
   </si>
   <si>
+    <t xml:space="preserve">PPT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cavaties Position</t>
   </si>
   <si>
@@ -481,6 +464,9 @@
   </si>
   <si>
     <t xml:space="preserve">WHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BTT3</t>
   </si>
   <si>
     <t xml:space="preserve">Decoy numbers</t>
@@ -551,7 +537,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -627,19 +613,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -940,7 +913,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1297,11 +1270,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1313,71 +1286,79 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1385,71 +1366,71 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1457,51 +1438,47 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1509,23 +1486,23 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1533,15 +1510,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1549,7 +1526,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1633,8 +1610,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4678,20 +4655,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:AMI29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+      <selection pane="topLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="89" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="89" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="4" style="89" width="10.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="10" style="89" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="89" width="10.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="9" style="89" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="89" width="10.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="14" style="89" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1023" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4714,9 +4694,8 @@
       <c r="O1" s="90"/>
       <c r="P1" s="90"/>
       <c r="Q1" s="90"/>
-      <c r="R1" s="90"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="90"/>
       <c r="B2" s="91"/>
       <c r="C2" s="90"/>
@@ -4734,9 +4713,8 @@
       <c r="O2" s="90"/>
       <c r="P2" s="90"/>
       <c r="Q2" s="90"/>
-      <c r="R2" s="90"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="90"/>
       <c r="B3" s="91"/>
       <c r="C3" s="92" t="s">
@@ -4750,17 +4728,16 @@
       <c r="G3" s="92"/>
       <c r="H3" s="92"/>
       <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
+      <c r="J3" s="90"/>
       <c r="K3" s="90"/>
       <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
+      <c r="M3" s="109"/>
       <c r="N3" s="90"/>
       <c r="O3" s="90"/>
       <c r="P3" s="90"/>
       <c r="Q3" s="90"/>
-      <c r="R3" s="90"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="90"/>
       <c r="B4" s="91"/>
       <c r="C4" s="90"/>
@@ -4778,153 +4755,140 @@
       <c r="O4" s="90"/>
       <c r="P4" s="90"/>
       <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-    </row>
-    <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="90"/>
       <c r="B5" s="94"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="109" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="109" t="s">
+      <c r="D5" s="110" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="109" t="s">
+      <c r="F5" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="109" t="s">
-        <v>93</v>
-      </c>
-      <c r="H5" s="109" t="s">
-        <v>94</v>
-      </c>
-      <c r="I5" s="109" t="s">
-        <v>95</v>
-      </c>
-      <c r="J5" s="109" t="s">
+      <c r="G5" s="110" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="110" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="110" t="s">
         <v>60</v>
       </c>
+      <c r="J5" s="90"/>
       <c r="K5" s="90"/>
       <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
+      <c r="M5" s="111"/>
       <c r="N5" s="90"/>
       <c r="O5" s="90"/>
       <c r="P5" s="90"/>
       <c r="Q5" s="90"/>
-      <c r="R5" s="90"/>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="90"/>
       <c r="B6" s="106" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C6" s="97" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D6" s="99" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E6" s="99" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F6" s="99" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G6" s="99" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H6" s="99" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I6" s="99" t="s">
-        <v>98</v>
-      </c>
-      <c r="J6" s="99" t="s">
-        <v>98</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="J6" s="90"/>
       <c r="K6" s="90"/>
       <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
+      <c r="M6" s="102"/>
       <c r="N6" s="90"/>
       <c r="O6" s="90"/>
       <c r="P6" s="90"/>
       <c r="Q6" s="90"/>
-      <c r="R6" s="90"/>
-    </row>
-    <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="90"/>
       <c r="B7" s="106"/>
       <c r="C7" s="97" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D7" s="99" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E7" s="99" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F7" s="99" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G7" s="99" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H7" s="99" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I7" s="99" t="s">
-        <v>99</v>
-      </c>
-      <c r="J7" s="99" t="s">
-        <v>98</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="J7" s="90"/>
       <c r="K7" s="90"/>
       <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
+      <c r="M7" s="102"/>
       <c r="N7" s="90"/>
       <c r="O7" s="90"/>
       <c r="P7" s="90"/>
       <c r="Q7" s="90"/>
-      <c r="R7" s="90"/>
-    </row>
-    <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="90"/>
       <c r="B8" s="106"/>
       <c r="C8" s="97" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D8" s="99" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E8" s="99" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F8" s="99" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G8" s="99" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H8" s="99" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I8" s="99" t="s">
-        <v>99</v>
-      </c>
-      <c r="J8" s="99" t="s">
-        <v>98</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="J8" s="90"/>
       <c r="K8" s="90"/>
       <c r="L8" s="90"/>
-      <c r="M8" s="90"/>
+      <c r="M8" s="102"/>
       <c r="N8" s="90"/>
       <c r="O8" s="90"/>
       <c r="P8" s="90"/>
       <c r="Q8" s="90"/>
-      <c r="R8" s="90"/>
-    </row>
-    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="90"/>
       <c r="B9" s="100"/>
       <c r="C9" s="101"/>
@@ -4934,103 +4898,99 @@
       <c r="G9" s="102"/>
       <c r="H9" s="102"/>
       <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
+      <c r="J9" s="90"/>
       <c r="K9" s="90"/>
       <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
+      <c r="M9" s="102"/>
       <c r="N9" s="90"/>
       <c r="O9" s="90"/>
       <c r="P9" s="90"/>
       <c r="Q9" s="90"/>
-      <c r="R9" s="90"/>
-    </row>
-    <row r="10" s="89" customFormat="true" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="10" customFormat="false" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="90"/>
       <c r="B10" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="110" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" s="111" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="111" t="s">
-        <v>103</v>
-      </c>
-      <c r="F10" s="112" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" s="111" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" s="111" t="s">
-        <v>103</v>
-      </c>
-      <c r="I10" s="111" t="s">
-        <v>103</v>
-      </c>
-      <c r="J10" s="112" t="s">
-        <v>104</v>
-      </c>
+      <c r="C10" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="114" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="114" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="114" t="s">
+        <v>101</v>
+      </c>
+      <c r="I10" s="114" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10" s="90"/>
       <c r="K10" s="90"/>
       <c r="L10" s="90"/>
-      <c r="M10" s="90"/>
+      <c r="M10" s="115"/>
       <c r="N10" s="90"/>
       <c r="O10" s="90"/>
       <c r="P10" s="90"/>
       <c r="Q10" s="90"/>
-      <c r="R10" s="90"/>
-    </row>
-    <row r="11" s="89" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMI10" s="89"/>
+    </row>
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="90"/>
       <c r="B11" s="100"/>
-      <c r="C11" s="113"/>
-      <c r="D11" s="114"/>
-      <c r="E11" s="114"/>
-      <c r="F11" s="115"/>
-      <c r="G11" s="114"/>
-      <c r="H11" s="114"/>
-      <c r="I11" s="114"/>
-      <c r="J11" s="115"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="115"/>
+      <c r="H11" s="115"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="90"/>
       <c r="K11" s="90"/>
       <c r="L11" s="90"/>
-      <c r="M11" s="90"/>
+      <c r="M11" s="115"/>
       <c r="N11" s="90"/>
       <c r="O11" s="90"/>
       <c r="P11" s="90"/>
       <c r="Q11" s="90"/>
-      <c r="R11" s="90"/>
+      <c r="AMI11" s="89"/>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="90"/>
       <c r="B12" s="103" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="97" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="118"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
+      <c r="G12" s="119"/>
+      <c r="H12" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="97" t="s">
-        <v>105</v>
-      </c>
-      <c r="D12" s="116"/>
-      <c r="E12" s="117"/>
-      <c r="F12" s="117"/>
-      <c r="G12" s="117"/>
-      <c r="H12" s="118"/>
       <c r="I12" s="99" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" s="99" t="s">
-        <v>98</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="J12" s="90"/>
       <c r="K12" s="90"/>
       <c r="L12" s="90"/>
-      <c r="M12" s="90"/>
+      <c r="M12" s="102"/>
       <c r="N12" s="90"/>
       <c r="O12" s="90"/>
       <c r="P12" s="90"/>
       <c r="Q12" s="90"/>
-      <c r="R12" s="90"/>
-    </row>
-    <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="90"/>
       <c r="B13" s="107"/>
       <c r="C13" s="101"/>
@@ -5040,97 +5000,93 @@
       <c r="G13" s="102"/>
       <c r="H13" s="102"/>
       <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
+      <c r="J13" s="90"/>
       <c r="K13" s="90"/>
       <c r="L13" s="90"/>
-      <c r="M13" s="90"/>
+      <c r="M13" s="102"/>
       <c r="N13" s="90"/>
       <c r="O13" s="90"/>
       <c r="P13" s="90"/>
       <c r="Q13" s="90"/>
-      <c r="R13" s="90"/>
-    </row>
-    <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="90"/>
       <c r="B14" s="108" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="C14" s="97" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" s="119"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="121"/>
+        <v>105</v>
+      </c>
+      <c r="D14" s="120"/>
+      <c r="E14" s="121"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="99" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="122"/>
       <c r="I14" s="99" t="s">
-        <v>98</v>
-      </c>
-      <c r="J14" s="99" t="s">
-        <v>98</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="J14" s="90"/>
       <c r="K14" s="90"/>
       <c r="L14" s="90"/>
-      <c r="M14" s="90"/>
+      <c r="M14" s="102"/>
       <c r="N14" s="90"/>
       <c r="O14" s="90"/>
       <c r="P14" s="90"/>
       <c r="Q14" s="90"/>
-      <c r="R14" s="90"/>
-    </row>
-    <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="90"/>
       <c r="B15" s="108"/>
       <c r="C15" s="97" t="s">
-        <v>107</v>
-      </c>
-      <c r="D15" s="122"/>
-      <c r="E15" s="123"/>
-      <c r="F15" s="123"/>
-      <c r="G15" s="123"/>
-      <c r="H15" s="124"/>
+        <v>106</v>
+      </c>
+      <c r="D15" s="123"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="99" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="125"/>
       <c r="I15" s="99" t="s">
-        <v>98</v>
-      </c>
-      <c r="J15" s="99" t="s">
-        <v>98</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="J15" s="90"/>
       <c r="K15" s="90"/>
       <c r="L15" s="90"/>
-      <c r="M15" s="90"/>
+      <c r="M15" s="102"/>
       <c r="N15" s="90"/>
       <c r="O15" s="90"/>
       <c r="P15" s="90"/>
       <c r="Q15" s="90"/>
-      <c r="R15" s="90"/>
-    </row>
-    <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="90"/>
       <c r="B16" s="108"/>
       <c r="C16" s="97" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="125"/>
-      <c r="E16" s="126"/>
-      <c r="F16" s="126"/>
-      <c r="G16" s="126"/>
-      <c r="H16" s="127"/>
+        <v>107</v>
+      </c>
+      <c r="D16" s="126"/>
+      <c r="E16" s="127"/>
+      <c r="F16" s="127"/>
+      <c r="G16" s="99" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="128"/>
       <c r="I16" s="99" t="s">
-        <v>65</v>
-      </c>
-      <c r="J16" s="99" t="s">
-        <v>65</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="J16" s="90"/>
       <c r="K16" s="90"/>
       <c r="L16" s="90"/>
-      <c r="M16" s="90"/>
+      <c r="M16" s="102"/>
       <c r="N16" s="90"/>
       <c r="O16" s="90"/>
       <c r="P16" s="90"/>
       <c r="Q16" s="90"/>
-      <c r="R16" s="90"/>
-    </row>
-    <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="90"/>
       <c r="B17" s="91"/>
       <c r="C17" s="90"/>
@@ -5148,9 +5104,8 @@
       <c r="O17" s="90"/>
       <c r="P17" s="90"/>
       <c r="Q17" s="90"/>
-      <c r="R17" s="90"/>
-    </row>
-    <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="90"/>
       <c r="B18" s="91"/>
       <c r="C18" s="90"/>
@@ -5168,9 +5123,8 @@
       <c r="O18" s="90"/>
       <c r="P18" s="90"/>
       <c r="Q18" s="90"/>
-      <c r="R18" s="90"/>
-    </row>
-    <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="90"/>
       <c r="B19" s="91"/>
       <c r="C19" s="90"/>
@@ -5188,9 +5142,8 @@
       <c r="O19" s="90"/>
       <c r="P19" s="90"/>
       <c r="Q19" s="90"/>
-      <c r="R19" s="90"/>
-    </row>
-    <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="90"/>
       <c r="B20" s="91"/>
       <c r="C20" s="90"/>
@@ -5208,9 +5161,8 @@
       <c r="O20" s="90"/>
       <c r="P20" s="90"/>
       <c r="Q20" s="90"/>
-      <c r="R20" s="90"/>
-    </row>
-    <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="90"/>
       <c r="B21" s="91"/>
       <c r="C21" s="90"/>
@@ -5228,9 +5180,8 @@
       <c r="O21" s="90"/>
       <c r="P21" s="90"/>
       <c r="Q21" s="90"/>
-      <c r="R21" s="90"/>
-    </row>
-    <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="90"/>
       <c r="B22" s="91"/>
       <c r="C22" s="90"/>
@@ -5248,9 +5199,8 @@
       <c r="O22" s="90"/>
       <c r="P22" s="90"/>
       <c r="Q22" s="90"/>
-      <c r="R22" s="90"/>
-    </row>
-    <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="90"/>
       <c r="B23" s="91"/>
       <c r="C23" s="90"/>
@@ -5268,9 +5218,8 @@
       <c r="O23" s="90"/>
       <c r="P23" s="90"/>
       <c r="Q23" s="90"/>
-      <c r="R23" s="90"/>
-    </row>
-    <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="90"/>
       <c r="B24" s="91"/>
       <c r="C24" s="90"/>
@@ -5288,9 +5237,8 @@
       <c r="O24" s="90"/>
       <c r="P24" s="90"/>
       <c r="Q24" s="90"/>
-      <c r="R24" s="90"/>
-    </row>
-    <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="90"/>
       <c r="B25" s="91"/>
       <c r="C25" s="90"/>
@@ -5308,9 +5256,8 @@
       <c r="O25" s="90"/>
       <c r="P25" s="90"/>
       <c r="Q25" s="90"/>
-      <c r="R25" s="90"/>
-    </row>
-    <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="90"/>
       <c r="B26" s="91"/>
       <c r="C26" s="90"/>
@@ -5328,9 +5275,8 @@
       <c r="O26" s="90"/>
       <c r="P26" s="90"/>
       <c r="Q26" s="90"/>
-      <c r="R26" s="90"/>
-    </row>
-    <row r="27" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="90"/>
       <c r="B27" s="91"/>
       <c r="C27" s="90"/>
@@ -5348,9 +5294,8 @@
       <c r="O27" s="90"/>
       <c r="P27" s="90"/>
       <c r="Q27" s="90"/>
-      <c r="R27" s="90"/>
-    </row>
-    <row r="28" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="90"/>
       <c r="B28" s="91"/>
       <c r="C28" s="90"/>
@@ -5368,9 +5313,8 @@
       <c r="O28" s="90"/>
       <c r="P28" s="90"/>
       <c r="Q28" s="90"/>
-      <c r="R28" s="90"/>
-    </row>
-    <row r="29" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="90"/>
       <c r="B29" s="91"/>
       <c r="C29" s="90"/>
@@ -5388,11 +5332,10 @@
       <c r="O29" s="90"/>
       <c r="P29" s="90"/>
       <c r="Q29" s="90"/>
-      <c r="R29" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="D3:I3"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B14:B16"/>
   </mergeCells>
@@ -5426,729 +5369,729 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="128"/>
+      <c r="A1" s="129"/>
       <c r="B1" s="11"/>
-      <c r="C1" s="129" t="s">
+      <c r="C1" s="130" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="130" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="130" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="130" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="129" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="129" t="s">
+      <c r="H1" s="130" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="130" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="130" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="131" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="132" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="133" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="134" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="134" t="n">
         <v>5</v>
       </c>
-      <c r="F1" s="129" t="s">
+      <c r="F2" s="134" t="n">
         <v>6</v>
       </c>
-      <c r="G1" s="129" t="s">
-        <v>93</v>
-      </c>
-      <c r="H1" s="129" t="s">
+      <c r="G2" s="134" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" s="134" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" s="134" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" s="135" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="131"/>
+      <c r="B3" s="136" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="137" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="124" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="124" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="124" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="124" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="124" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="124" t="n">
+        <v>3</v>
+      </c>
+      <c r="J3" s="138" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="131"/>
+      <c r="B4" s="136" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="129" t="s">
+      <c r="C4" s="124" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="124" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="129" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="130" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="131" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="132" t="s">
+      <c r="E4" s="124" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="124" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="124" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="124" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="124" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4" s="138" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="131"/>
+      <c r="B5" s="136" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="124" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="124" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="124" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="124" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="124" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="124" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="124" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" s="138" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="131"/>
+      <c r="B6" s="139" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="124" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="140" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="140" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="140" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="140" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="140" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="140" t="s">
+        <v>97</v>
+      </c>
+      <c r="J6" s="141" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="131" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="132" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="134" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="133" t="n">
+      <c r="D7" s="134" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="134" t="n">
         <v>3</v>
       </c>
-      <c r="E2" s="133" t="n">
+      <c r="F7" s="134" t="n">
+        <v>4</v>
+      </c>
+      <c r="G7" s="134" t="n">
         <v>5</v>
       </c>
-      <c r="F2" s="133" t="n">
-        <v>6</v>
-      </c>
-      <c r="G2" s="133" t="n">
-        <v>6</v>
-      </c>
-      <c r="H2" s="133" t="n">
+      <c r="H7" s="134" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="134" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="135" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="131"/>
+      <c r="B8" s="142" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="143" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="143" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="143" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="144" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="143" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="143" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="143" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" s="145" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="131"/>
+      <c r="B9" s="139" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="140" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="140" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="140" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="140" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="141" t="n">
         <v>3</v>
       </c>
-      <c r="I2" s="133" t="n">
+    </row>
+    <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="146" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="132" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="134" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="134" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" s="134" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="134"/>
+      <c r="J10" s="135" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="146"/>
+      <c r="B11" s="139" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="140" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="140" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="140" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="141" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="129"/>
+      <c r="D12" s="129"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="129"/>
+      <c r="G12" s="129"/>
+      <c r="H12" s="129"/>
+      <c r="I12" s="129"/>
+      <c r="J12" s="129"/>
+    </row>
+    <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="147" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="132" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="134" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="134" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="135" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="147"/>
+      <c r="B14" s="136" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="124" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="124" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="124" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="124" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="124" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="124" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="124" t="n">
         <v>3</v>
       </c>
-      <c r="J2" s="134" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="130"/>
-      <c r="B3" s="135" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="136" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="123" t="n">
+      <c r="J14" s="138" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="147"/>
+      <c r="B15" s="136" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="124" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="124" t="s">
+        <v>95</v>
+      </c>
+      <c r="J15" s="124" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="147"/>
+      <c r="B16" s="148" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="149" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="149" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="123" t="n">
+      <c r="E16" s="149" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="149" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="149" t="n">
         <v>3</v>
       </c>
-      <c r="F3" s="123" t="n">
+      <c r="H16" s="149"/>
+      <c r="I16" s="149"/>
+      <c r="J16" s="150" t="n">
         <v>3</v>
       </c>
-      <c r="G3" s="123" t="n">
-        <v>3</v>
-      </c>
-      <c r="H3" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="123" t="n">
-        <v>3</v>
-      </c>
-      <c r="J3" s="137" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="130"/>
-      <c r="B4" s="135" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="123" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="123" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" s="123" t="s">
-        <v>98</v>
-      </c>
-      <c r="F4" s="123" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="123" t="s">
-        <v>98</v>
-      </c>
-      <c r="H4" s="123" t="s">
-        <v>99</v>
-      </c>
-      <c r="I4" s="123" t="s">
-        <v>98</v>
-      </c>
-      <c r="J4" s="137" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="130"/>
-      <c r="B5" s="135" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="123" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" s="123" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="123" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="123" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="123" t="s">
-        <v>98</v>
-      </c>
-      <c r="H5" s="123" t="s">
-        <v>99</v>
-      </c>
-      <c r="I5" s="123" t="s">
-        <v>99</v>
-      </c>
-      <c r="J5" s="137" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="130"/>
-      <c r="B6" s="138" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="123" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="139" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="139" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" s="139" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" s="139" t="s">
-        <v>99</v>
-      </c>
-      <c r="H6" s="139" t="s">
-        <v>99</v>
-      </c>
-      <c r="I6" s="139" t="s">
-        <v>99</v>
-      </c>
-      <c r="J6" s="140" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="130" t="s">
-        <v>112</v>
-      </c>
-      <c r="B7" s="131" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="133" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="133" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" s="133" t="n">
-        <v>3</v>
-      </c>
-      <c r="F7" s="133" t="n">
-        <v>4</v>
-      </c>
-      <c r="G7" s="133" t="n">
-        <v>5</v>
-      </c>
-      <c r="H7" s="133" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" s="133" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="134" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="130"/>
-      <c r="B8" s="141" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="142" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="142" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" s="142" t="s">
-        <v>103</v>
-      </c>
-      <c r="F8" s="143" t="s">
-        <v>104</v>
-      </c>
-      <c r="G8" s="142" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="142" t="s">
-        <v>103</v>
-      </c>
-      <c r="I8" s="142" t="s">
-        <v>103</v>
-      </c>
-      <c r="J8" s="144" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="130"/>
-      <c r="B9" s="138" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="139" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="139" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="139" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="139" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="139" t="n">
-        <v>2</v>
-      </c>
-      <c r="H9" s="139" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="139" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="140" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="145" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="131" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="133" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="133" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="133" t="n">
-        <v>2</v>
-      </c>
-      <c r="F10" s="133" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="133" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="133" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="133"/>
-      <c r="J10" s="134" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="145"/>
-      <c r="B11" s="138" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="139" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="139" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="139" t="n">
-        <v>2</v>
-      </c>
-      <c r="F11" s="139" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="139" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="139" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="139" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="140" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="128"/>
-      <c r="D12" s="128"/>
-      <c r="E12" s="128"/>
-      <c r="F12" s="128"/>
-      <c r="G12" s="128"/>
-      <c r="H12" s="128"/>
-      <c r="I12" s="128"/>
-      <c r="J12" s="128"/>
-    </row>
-    <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="146" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="131" t="s">
-        <v>114</v>
-      </c>
-      <c r="C13" s="133" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="133" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="133" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="133" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="133" t="n">
-        <v>2</v>
-      </c>
-      <c r="H13" s="133" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="133" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="134" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="146"/>
-      <c r="B14" s="135" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="123" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="123" t="n">
-        <v>3</v>
-      </c>
-      <c r="J14" s="137" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="146"/>
-      <c r="B15" s="135" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="123" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" s="123"/>
-      <c r="E15" s="123"/>
-      <c r="F15" s="123"/>
-      <c r="G15" s="123"/>
-      <c r="H15" s="123"/>
-      <c r="I15" s="123" t="s">
-        <v>98</v>
-      </c>
-      <c r="J15" s="123" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="146"/>
-      <c r="B16" s="147" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" s="148" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="148" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="148" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="148" t="n">
-        <v>3</v>
-      </c>
-      <c r="H16" s="148"/>
-      <c r="I16" s="148"/>
-      <c r="J16" s="149" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="150" t="s">
+      <c r="A17" s="151" t="s">
         <v>77</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="128" t="s">
+      <c r="C17" s="129" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="128" t="n">
+      <c r="D17" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="E17" s="128" t="n">
+      <c r="E17" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="F17" s="128" t="n">
+      <c r="F17" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="128" t="n">
+      <c r="G17" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="H17" s="128" t="n">
+      <c r="H17" s="129" t="n">
         <v>3</v>
       </c>
-      <c r="I17" s="128" t="n">
+      <c r="I17" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="J17" s="128" t="n">
+      <c r="J17" s="129" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="150"/>
+      <c r="A18" s="151"/>
       <c r="B18" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="128" t="s">
+      <c r="C18" s="129" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="128" t="n">
+      <c r="D18" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="E18" s="128" t="n">
+      <c r="E18" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="F18" s="128" t="n">
+      <c r="F18" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="G18" s="128" t="n">
+      <c r="G18" s="129" t="n">
         <v>1</v>
       </c>
-      <c r="H18" s="128" t="n">
+      <c r="H18" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="128" t="n">
+      <c r="I18" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="J18" s="128" t="n">
+      <c r="J18" s="129" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="150"/>
+      <c r="A19" s="151"/>
       <c r="B19" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="128" t="s">
+      <c r="C19" s="129" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="128" t="n">
+      <c r="D19" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="E19" s="128" t="n">
+      <c r="E19" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="F19" s="128" t="n">
+      <c r="F19" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="G19" s="128" t="n">
+      <c r="G19" s="129" t="n">
         <v>2</v>
       </c>
-      <c r="H19" s="128" t="n">
+      <c r="H19" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I19" s="128" t="n">
+      <c r="I19" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="J19" s="128" t="n">
+      <c r="J19" s="129" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="150"/>
+      <c r="A20" s="151"/>
       <c r="B20" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="128" t="s">
+      <c r="C20" s="129" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="128" t="n">
+      <c r="D20" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="E20" s="128" t="n">
+      <c r="E20" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="F20" s="128" t="n">
+      <c r="F20" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="G20" s="128" t="n">
+      <c r="G20" s="129" t="n">
         <v>2</v>
       </c>
-      <c r="H20" s="128" t="n">
+      <c r="H20" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="128" t="n">
+      <c r="I20" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="J20" s="128" t="n">
+      <c r="J20" s="129" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="150"/>
+      <c r="A21" s="151"/>
       <c r="B21" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="128" t="s">
+      <c r="C21" s="129" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="128" t="n">
+      <c r="D21" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="E21" s="128" t="n">
+      <c r="E21" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="F21" s="128" t="n">
+      <c r="F21" s="129" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="128" t="n">
+      <c r="G21" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="H21" s="128" t="n">
+      <c r="H21" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="I21" s="128" t="n">
+      <c r="I21" s="129" t="n">
         <v>0</v>
       </c>
-      <c r="J21" s="128" t="n">
+      <c r="J21" s="129" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="150"/>
-      <c r="B22" s="151" t="s">
+      <c r="A22" s="151"/>
+      <c r="B22" s="152" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="152" t="s">
+      <c r="C22" s="153" t="s">
         <v>118</v>
       </c>
-      <c r="D22" s="152" t="n">
+      <c r="D22" s="153" t="n">
         <v>0</v>
       </c>
-      <c r="E22" s="152" t="n">
+      <c r="E22" s="153" t="n">
         <v>1</v>
       </c>
-      <c r="F22" s="152" t="n">
+      <c r="F22" s="153" t="n">
         <v>2</v>
       </c>
-      <c r="G22" s="152" t="n">
+      <c r="G22" s="153" t="n">
         <v>3</v>
       </c>
-      <c r="H22" s="152"/>
-      <c r="I22" s="152"/>
-      <c r="J22" s="152" t="n">
+      <c r="H22" s="153"/>
+      <c r="I22" s="153"/>
+      <c r="J22" s="153" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="150"/>
+      <c r="A23" s="151"/>
       <c r="B23" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="123" t="s">
+      <c r="C23" s="124" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="128"/>
-      <c r="E23" s="128"/>
-      <c r="F23" s="128"/>
-      <c r="G23" s="128"/>
-      <c r="H23" s="128"/>
-      <c r="I23" s="128" t="s">
-        <v>98</v>
-      </c>
-      <c r="J23" s="128" t="s">
-        <v>98</v>
+      <c r="D23" s="129"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="129"/>
+      <c r="G23" s="129"/>
+      <c r="H23" s="129"/>
+      <c r="I23" s="129" t="s">
+        <v>95</v>
+      </c>
+      <c r="J23" s="129" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="150"/>
+      <c r="A24" s="151"/>
       <c r="B24" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="123" t="s">
+      <c r="C24" s="124" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="128"/>
-      <c r="E24" s="128"/>
-      <c r="F24" s="128"/>
-      <c r="G24" s="128"/>
-      <c r="H24" s="128"/>
-      <c r="I24" s="128" t="s">
-        <v>98</v>
-      </c>
-      <c r="J24" s="128" t="s">
-        <v>98</v>
+      <c r="D24" s="129"/>
+      <c r="E24" s="129"/>
+      <c r="F24" s="129"/>
+      <c r="G24" s="129"/>
+      <c r="H24" s="129"/>
+      <c r="I24" s="129" t="s">
+        <v>95</v>
+      </c>
+      <c r="J24" s="129" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="150"/>
+      <c r="A25" s="151"/>
       <c r="B25" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="123" t="s">
+      <c r="C25" s="124" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="128"/>
-      <c r="E25" s="128"/>
-      <c r="F25" s="128"/>
-      <c r="G25" s="128"/>
-      <c r="H25" s="128"/>
-      <c r="I25" s="128" t="s">
-        <v>99</v>
-      </c>
-      <c r="J25" s="128" t="s">
-        <v>99</v>
+      <c r="D25" s="129"/>
+      <c r="E25" s="129"/>
+      <c r="F25" s="129"/>
+      <c r="G25" s="129"/>
+      <c r="H25" s="129"/>
+      <c r="I25" s="129" t="s">
+        <v>97</v>
+      </c>
+      <c r="J25" s="129" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="128"/>
-      <c r="D26" s="128"/>
-      <c r="E26" s="128"/>
-      <c r="F26" s="128"/>
-      <c r="G26" s="128"/>
-      <c r="H26" s="128"/>
-      <c r="I26" s="128"/>
-      <c r="J26" s="128"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="129"/>
+      <c r="F26" s="129"/>
+      <c r="G26" s="129"/>
+      <c r="H26" s="129"/>
+      <c r="I26" s="129"/>
+      <c r="J26" s="129"/>
     </row>
     <row r="27" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="128" t="s">
+      <c r="C27" s="129" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="128" t="s">
+      <c r="D27" s="129" t="s">
         <v>128</v>
       </c>
-      <c r="E27" s="128" t="s">
+      <c r="E27" s="129" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="128" t="s">
+      <c r="F27" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="128" t="s">
+      <c r="G27" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="H27" s="128" t="s">
+      <c r="H27" s="129" t="s">
         <v>84</v>
       </c>
-      <c r="I27" s="128" t="s">
+      <c r="I27" s="129" t="s">
         <v>84</v>
       </c>
-      <c r="J27" s="128" t="s">
+      <c r="J27" s="129" t="s">
         <v>129</v>
       </c>
     </row>

</xml_diff>